<commit_message>
Task-2 | Queries Added
</commit_message>
<xml_diff>
--- a/ECS/users/Users.xlsx
+++ b/ECS/users/Users.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
   <si>
     <t>ID</t>
   </si>
@@ -39,6 +39,9 @@
     <t>Role</t>
   </si>
   <si>
+    <t>Password</t>
+  </si>
+  <si>
     <t>Ali</t>
   </si>
   <si>
@@ -54,6 +57,9 @@
     <t>Customer</t>
   </si>
   <si>
+    <t>ali123</t>
+  </si>
+  <si>
     <t>Qasim</t>
   </si>
   <si>
@@ -66,6 +72,24 @@
     <t>Lahore</t>
   </si>
   <si>
+    <t>qasim123</t>
+  </si>
+  <si>
+    <t>Abdullah</t>
+  </si>
+  <si>
+    <t>abdullah</t>
+  </si>
+  <si>
+    <t>abdullah@gmail.com</t>
+  </si>
+  <si>
+    <t>Karachi</t>
+  </si>
+  <si>
+    <t>abdullah123</t>
+  </si>
+  <si>
     <t>Arslan</t>
   </si>
   <si>
@@ -75,12 +99,12 @@
     <t>arslan@gmail.com</t>
   </si>
   <si>
-    <t>Karachi</t>
-  </si>
-  <si>
     <t>AppAdmin</t>
   </si>
   <si>
+    <t>arslan123</t>
+  </si>
+  <si>
     <t>Umer</t>
   </si>
   <si>
@@ -90,6 +114,9 @@
     <t>umer@gmail.com</t>
   </si>
   <si>
+    <t>umer123</t>
+  </si>
+  <si>
     <t>Muhammad</t>
   </si>
   <si>
@@ -102,10 +129,16 @@
     <t>ShopAdmin</t>
   </si>
   <si>
+    <t>ahmad123</t>
+  </si>
+  <si>
     <t>muhammad</t>
   </si>
   <si>
     <t>mali@gmail.com</t>
+  </si>
+  <si>
+    <t>muhammad123</t>
   </si>
 </sst>
 </file>
@@ -395,28 +428,34 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
         <v>1.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="1">
         <v>3.12345677E8</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3">
@@ -424,25 +463,54 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1">
         <v>3.45899903E8</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -485,31 +553,37 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
         <v>3.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F2" s="1">
         <v>3.1235567732E10</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3">
@@ -517,25 +591,28 @@
         <v>4.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="F3" s="1">
         <v>3.4389990222E10</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -578,31 +655,37 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
         <v>5.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="F2" s="1">
         <v>3.1535567732E10</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3">
@@ -610,25 +693,28 @@
         <v>6.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F3" s="1">
         <v>3.438999022E10</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>